<commit_message>
Atualização das tabelas para o bok splot
</commit_message>
<xml_diff>
--- a/Algoritmo_Rota/Planilhas/A_Estrela_Euclidiano/PLN_13_10.xlsx
+++ b/Algoritmo_Rota/Planilhas/A_Estrela_Euclidiano/PLN_13_10.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,20 +424,25 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Qtd_Nós</t>
+          <t>Índice</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
-        <is>
-          <t>Ativos</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
         <is>
           <t>Distancia</t>
         </is>
       </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>max</t>
+        </is>
+      </c>
       <c r="D1" t="inlineStr">
+        <is>
+          <t>min</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
         <is>
           <t>Tempo</t>
         </is>
@@ -445,16 +450,172 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>10</v>
+        <v>1283.133333333333</v>
       </c>
       <c r="C2" t="n">
-        <v>1285</v>
+        <v>1440</v>
       </c>
       <c r="D2" t="n">
-        <v>0.02776360511779785</v>
+        <v>1223</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.02868414719899496</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="n">
+        <v>1327.433333333333</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1436</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1272</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.02877468268076579</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>1304.6</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1451</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1224</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.03174591859181722</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>1313.033333333333</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1438</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1272</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.02855827808380127</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>1285.366666666667</v>
+      </c>
+      <c r="C6" t="n">
+        <v>1389</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1221</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.02888263066609701</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>1178</v>
+      </c>
+      <c r="C7" t="n">
+        <v>1316</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1068</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.02907733917236328</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>1147.9</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1365</v>
+      </c>
+      <c r="D8" t="n">
+        <v>1057</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.02906942367553711</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>1131.466666666667</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1220</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1068</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.02921895980834961</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>1260.9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>1375</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1221</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.02915266354878743</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>1152.9</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1390</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1057</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.02910596529642741</v>
       </c>
     </row>
   </sheetData>

</xml_diff>